<commit_message>
settings.py file email updation
</commit_message>
<xml_diff>
--- a/static/weather.xlsx
+++ b/static/weather.xlsx
@@ -466,10 +466,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C2">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -480,7 +480,7 @@
         <v>302.59</v>
       </c>
       <c r="C3">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -488,10 +488,10 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>305.05</v>
+        <v>305.58</v>
       </c>
       <c r="C4">
-        <v>305.05</v>
+        <v>305.58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -502,7 +502,7 @@
         <v>302.59</v>
       </c>
       <c r="C5">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -510,10 +510,10 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>304.15</v>
+        <v>304.82</v>
       </c>
       <c r="C6">
-        <v>304.82</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -521,10 +521,10 @@
         <v>8</v>
       </c>
       <c r="B7">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C7">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -532,10 +532,10 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <v>305.34</v>
+        <v>305.84</v>
       </c>
       <c r="C8">
-        <v>305.34</v>
+        <v>305.84</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -543,10 +543,10 @@
         <v>10</v>
       </c>
       <c r="B9">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C9">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -557,7 +557,7 @@
         <v>302.59</v>
       </c>
       <c r="C10">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -565,10 +565,10 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C11">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -576,10 +576,10 @@
         <v>13</v>
       </c>
       <c r="B12">
-        <v>305.46</v>
+        <v>306.12</v>
       </c>
       <c r="C12">
-        <v>305.46</v>
+        <v>306.12</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -590,7 +590,7 @@
         <v>302.59</v>
       </c>
       <c r="C13">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -598,10 +598,10 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C14">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -609,10 +609,10 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C15">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -623,7 +623,7 @@
         <v>302.59</v>
       </c>
       <c r="C16">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -631,10 +631,10 @@
         <v>18</v>
       </c>
       <c r="B17">
-        <v>304.34</v>
+        <v>305.51</v>
       </c>
       <c r="C17">
-        <v>304.34</v>
+        <v>305.51</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -645,7 +645,7 @@
         <v>302.59</v>
       </c>
       <c r="C18">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -653,10 +653,10 @@
         <v>20</v>
       </c>
       <c r="B19">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C19">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -664,10 +664,10 @@
         <v>21</v>
       </c>
       <c r="B20">
-        <v>305.19</v>
+        <v>305.72</v>
       </c>
       <c r="C20">
-        <v>305.19</v>
+        <v>305.72</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -675,10 +675,10 @@
         <v>22</v>
       </c>
       <c r="B21">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C21">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -686,10 +686,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C22">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -697,10 +697,10 @@
         <v>24</v>
       </c>
       <c r="B23">
-        <v>305.76</v>
+        <v>306.08</v>
       </c>
       <c r="C23">
-        <v>305.76</v>
+        <v>306.08</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -711,7 +711,7 @@
         <v>302.59</v>
       </c>
       <c r="C24">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -719,10 +719,10 @@
         <v>26</v>
       </c>
       <c r="B25">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C25">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -730,10 +730,10 @@
         <v>27</v>
       </c>
       <c r="B26">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C26">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -741,10 +741,10 @@
         <v>28</v>
       </c>
       <c r="B27">
-        <v>302.59</v>
+        <v>302.04</v>
       </c>
       <c r="C27">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -752,10 +752,10 @@
         <v>29</v>
       </c>
       <c r="B28">
-        <v>302.59</v>
+        <v>302.04</v>
       </c>
       <c r="C28">
-        <v>304.82</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -763,10 +763,10 @@
         <v>30</v>
       </c>
       <c r="B29">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
       <c r="C29">
-        <v>304.15</v>
+        <v>306.15</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -777,7 +777,7 @@
         <v>302.59</v>
       </c>
       <c r="C30">
-        <v>303.15</v>
+        <v>305.15</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -788,7 +788,7 @@
         <v>302.59</v>
       </c>
       <c r="C31">
-        <v>303.15</v>
+        <v>305.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>